<commit_message>
Add utility views for production, icons
</commit_message>
<xml_diff>
--- a/production.xlsx
+++ b/production.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VS Projects\anno-assist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87147245-2741-41F2-9143-C1CB0FB7EADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752B6E08-AB3D-427A-9A3B-E9547A17C250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{831166C9-CADB-4C15-A02D-BEA01D63DA5D}"/>
   </bookViews>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AB8F55-71A6-49E8-87C2-65462365D625}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,7 +2711,7 @@
         <v>37</v>
       </c>
       <c r="F46">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="G46" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2731,11 +2731,11 @@
       </c>
       <c r="K46" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>"rate_B":0.5</v>
+        <v>"rate_B":0.8</v>
       </c>
       <c r="L46" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>"meat":{"output":24, "input_A":"cattle", "rate_A":1, "input_B":"salt", "rate_B":0.5}</v>
+        <v>"meat":{"output":24, "input_A":"cattle", "rate_A":1, "input_B":"salt", "rate_B":0.8}</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -3489,7 +3489,7 @@
     <row r="64" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L64" s="3" t="str">
         <f>_xlfn.TEXTJOIN(","&amp;CHAR(32),TRUE,L2:L63)</f>
-        <v>"spices":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "cider":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "hemp":{"output":60, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "almonds":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "wheat":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "herbs":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "grapes":{"output":90, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "wax":{"output":90, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "coffee_beans":{"output":60, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "roses":{"output":120, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "sugar_cane":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "indigo":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "silk":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "dates":{"output":20, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "milk":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "cattle":{"output":48, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "hides":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "clay":{"output":50, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "wood":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "potash":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "coal":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "fish":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "quartz":{"output":45, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "stone":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "iron_ore":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "brine":{"output":15, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "copper":{"output":45, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "gold_ore":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "furs":{"output":24, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "pearls":{"output":60, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "leather":{"output":15, "input_A":"hides", "rate_A":1, "input_B":"salt", "rate_B":0.5}, "sugar":{"output":15, "input_A":"sugar_cane", "rate_A":1, "input_B":null, "rate_B":null}, "paper":{"output":20, "input_A":"wood", "rate_A":1, "input_B":null, "rate_B":null}, "furcoats":{"output":24, "input_A":"furs", "rate_A":1, "input_B":"salt", "rate_B":0.53}, "linen":{"output":30, "input_A":"hemp", "rate_A":1, "input_B":null, "rate_B":null}, "tools":{"output":30, "input_A":"iron", "rate_A":0.5, "input_B":null, "rate_B":null}, "mosaic":{"output":25, "input_A":"clay", "rate_A":1, "input_B":"quartz", "rate_B":0.5}, "flour":{"output":15, "input_A":"wheat", "rate_A":1, "input_B":null, "rate_B":null}, "bread":{"output":15, "input_A":"flour", "rate_A":1, "input_B":null, "rate_B":null}, "beer":{"output":40, "input_A":"herbs", "rate_A":1.333, "input_B":"wheat", "rate_B":1.333}, "iron":{"output":30, "input_A":"iron_ore", "rate_A":1, "input_B":"coal", "rate_B":1}, "rope":{"output":30, "input_A":"hemp", "rate_A":0.5, "input_B":null, "rate_B":null}, "weapons":{"output":30, "input_A":"iron", "rate_A":1, "input_B":null, "rate_B":null}, "salt":{"output":15, "input_A":"brine", "rate_A":1, "input_B":"coal", "rate_B":0.5}, "meat":{"output":24, "input_A":"cattle", "rate_A":1, "input_B":"salt", "rate_B":0.5}, "barrels":{"output":30, "input_A":"wood", "rate_A":0.5, "input_B":"iron", "rate_B":0.5}, "wine":{"output":30, "input_A":"grapes", "rate_A":1, "input_B":"barrels", "rate_B":1}, "coffee":{"output":60, "input_A":"coffee_beans", "rate_A":2, "input_B":null, "rate_B":null}, "war_machines":{"output":40, "input_A":"wood", "rate_A":2, "input_B":"rope", "rate_B":2}, "brass":{"output":45, "input_A":"copper", "rate_A":1, "input_B":"coal", "rate_B":1}, "glasses":{"output":30, "input_A":"brass", "rate_A":0.5, "input_B":"quartz", "rate_B":0.5}, "candles":{"output":45, "input_A":"wax", "rate_A":1, "input_B":"hemp", "rate_B":0.75}, "candlestick":{"output":30, "input_A":"brass", "rate_A":0.5, "input_B":"candles", "rate_B":1}, "perfume":{"output":60, "input_A":"roses", "rate_A":1.5, "input_B":null, "rate_B":null}, "marzipan":{"output":15, "input_A":"almonds", "rate_A":1, "input_B":"sugar", "rate_B":1}, "brocade":{"output":20, "input_A":"silk", "rate_A":1, "input_B":"gold", "rate_B":0.5}, "carpets":{"output":40, "input_A":"silk", "rate_A":1, "input_B":"indigo", "rate_B":1}, "gold":{"output":40, "input_A":"gold_ore", "rate_A":1, "input_B":"coal", "rate_B":1}, "necklaces":{"output":60, "input_A":"pearls", "rate_A":1, "input_B":null, "rate_B":null}, "cannons":{"output":60, "input_A":"iron", "rate_A":1.5, "input_B":"wood", "rate_B":3}, "books":{"output":20, "input_A":"paper", "rate_A":0.5, "input_B":"indigo", "rate_B":1}, "glass":{"output":60, "input_A":"potash", "rate_A":1, "input_B":"quartz", "rate_B":0.5}</v>
+        <v>"spices":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "cider":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "hemp":{"output":60, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "almonds":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "wheat":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "herbs":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "grapes":{"output":90, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "wax":{"output":90, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "coffee_beans":{"output":60, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "roses":{"output":120, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "sugar_cane":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "indigo":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "silk":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "dates":{"output":20, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "milk":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "cattle":{"output":48, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "hides":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "clay":{"output":50, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "wood":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "potash":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "coal":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "fish":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "quartz":{"output":45, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "stone":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "iron_ore":{"output":30, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "brine":{"output":15, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "copper":{"output":45, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "gold_ore":{"output":40, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "furs":{"output":24, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "pearls":{"output":60, "input_A":null, "rate_A":null, "input_B":null, "rate_B":null}, "leather":{"output":15, "input_A":"hides", "rate_A":1, "input_B":"salt", "rate_B":0.5}, "sugar":{"output":15, "input_A":"sugar_cane", "rate_A":1, "input_B":null, "rate_B":null}, "paper":{"output":20, "input_A":"wood", "rate_A":1, "input_B":null, "rate_B":null}, "furcoats":{"output":24, "input_A":"furs", "rate_A":1, "input_B":"salt", "rate_B":0.53}, "linen":{"output":30, "input_A":"hemp", "rate_A":1, "input_B":null, "rate_B":null}, "tools":{"output":30, "input_A":"iron", "rate_A":0.5, "input_B":null, "rate_B":null}, "mosaic":{"output":25, "input_A":"clay", "rate_A":1, "input_B":"quartz", "rate_B":0.5}, "flour":{"output":15, "input_A":"wheat", "rate_A":1, "input_B":null, "rate_B":null}, "bread":{"output":15, "input_A":"flour", "rate_A":1, "input_B":null, "rate_B":null}, "beer":{"output":40, "input_A":"herbs", "rate_A":1.333, "input_B":"wheat", "rate_B":1.333}, "iron":{"output":30, "input_A":"iron_ore", "rate_A":1, "input_B":"coal", "rate_B":1}, "rope":{"output":30, "input_A":"hemp", "rate_A":0.5, "input_B":null, "rate_B":null}, "weapons":{"output":30, "input_A":"iron", "rate_A":1, "input_B":null, "rate_B":null}, "salt":{"output":15, "input_A":"brine", "rate_A":1, "input_B":"coal", "rate_B":0.5}, "meat":{"output":24, "input_A":"cattle", "rate_A":1, "input_B":"salt", "rate_B":0.8}, "barrels":{"output":30, "input_A":"wood", "rate_A":0.5, "input_B":"iron", "rate_B":0.5}, "wine":{"output":30, "input_A":"grapes", "rate_A":1, "input_B":"barrels", "rate_B":1}, "coffee":{"output":60, "input_A":"coffee_beans", "rate_A":2, "input_B":null, "rate_B":null}, "war_machines":{"output":40, "input_A":"wood", "rate_A":2, "input_B":"rope", "rate_B":2}, "brass":{"output":45, "input_A":"copper", "rate_A":1, "input_B":"coal", "rate_B":1}, "glasses":{"output":30, "input_A":"brass", "rate_A":0.5, "input_B":"quartz", "rate_B":0.5}, "candles":{"output":45, "input_A":"wax", "rate_A":1, "input_B":"hemp", "rate_B":0.75}, "candlestick":{"output":30, "input_A":"brass", "rate_A":0.5, "input_B":"candles", "rate_B":1}, "perfume":{"output":60, "input_A":"roses", "rate_A":1.5, "input_B":null, "rate_B":null}, "marzipan":{"output":15, "input_A":"almonds", "rate_A":1, "input_B":"sugar", "rate_B":1}, "brocade":{"output":20, "input_A":"silk", "rate_A":1, "input_B":"gold", "rate_B":0.5}, "carpets":{"output":40, "input_A":"silk", "rate_A":1, "input_B":"indigo", "rate_B":1}, "gold":{"output":40, "input_A":"gold_ore", "rate_A":1, "input_B":"coal", "rate_B":1}, "necklaces":{"output":60, "input_A":"pearls", "rate_A":1, "input_B":null, "rate_B":null}, "cannons":{"output":60, "input_A":"iron", "rate_A":1.5, "input_B":"wood", "rate_B":3}, "books":{"output":20, "input_A":"paper", "rate_A":0.5, "input_B":"indigo", "rate_B":1}, "glass":{"output":60, "input_A":"potash", "rate_A":1, "input_B":"quartz", "rate_B":0.5}</v>
       </c>
     </row>
     <row r="65" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>